<commit_message>
Added New Test Cases for Deals Page
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dudha\Desktop\QA\Selenium_WorkSpace\FreeCRMTest\src\main\java\com\crm\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27BD4A3-88F3-40B4-B880-5676105C0154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27764036-C365-4F7A-AC38-899C3595B99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3344554C-853B-4DE3-BE7E-11E8D351355B}"/>
+    <workbookView xWindow="15180" yWindow="1290" windowWidth="11805" windowHeight="9225" activeTab="1" xr2:uid="{3344554C-853B-4DE3-BE7E-11E8D351355B}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
+    <sheet name="deals" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>title</t>
   </si>
@@ -82,6 +83,9 @@
   </si>
   <si>
     <t>Facebook</t>
+  </si>
+  <si>
+    <t>abcd</t>
   </si>
 </sst>
 </file>
@@ -442,7 +446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD5E192-A3B8-4C59-BA3B-7362940A2F39}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
@@ -511,4 +515,29 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70135500-022E-4719-8CD4-2C476CE641AC}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>